<commit_message>
we run some test cases
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/employeedata.xlsx
+++ b/src/test/resources/testdata/employeedata.xlsx
@@ -3,22 +3,23 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22730"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{C08A74AF-999E-4EAE-AD5E-009879773A3A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{858D9DD3-EB99-4645-93F0-F0B2EF2A250E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="23112" windowHeight="13224" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2688" yWindow="2688" windowWidth="23088" windowHeight="13224" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="negativelogindata" sheetId="2" r:id="rId1"/>
     <sheet name="addEmpdata" sheetId="1" r:id="rId2"/>
     <sheet name="positivelogindata" sheetId="3" r:id="rId3"/>
+    <sheet name="personnalDetails" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A4:K20"/>
+  <oleSize ref="A1:D17"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="89">
   <si>
     <t>UserNames</t>
   </si>
@@ -183,6 +184,108 @@
   </si>
   <si>
     <t>Hum@nhrm123</t>
+  </si>
+  <si>
+    <t>License Expiry Date</t>
+  </si>
+  <si>
+    <t>driver licence number</t>
+  </si>
+  <si>
+    <t>Ssn number</t>
+  </si>
+  <si>
+    <t>Other id</t>
+  </si>
+  <si>
+    <t>Nick name</t>
+  </si>
+  <si>
+    <t>Military service</t>
+  </si>
+  <si>
+    <t>Sin number</t>
+  </si>
+  <si>
+    <t>Marital Status</t>
+  </si>
+  <si>
+    <t>Nationality</t>
+  </si>
+  <si>
+    <t>Smoker</t>
+  </si>
+  <si>
+    <t>dat of birth</t>
+  </si>
+  <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>1994-Mar-15</t>
+  </si>
+  <si>
+    <t>A66666325</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Single</t>
+  </si>
+  <si>
+    <t>Algerian</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>male</t>
+  </si>
+  <si>
+    <t>B44445558</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Married </t>
+  </si>
+  <si>
+    <t>American</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>female</t>
+  </si>
+  <si>
+    <t>J448885285</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Armenian</t>
+  </si>
+  <si>
+    <t>Y4885626555</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>Bahamian</t>
   </si>
 </sst>
 </file>
@@ -515,8 +618,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17:B18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -614,8 +717,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -846,4 +949,221 @@
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:L5"/>
+  <sheetViews>
+    <sheetView topLeftCell="H6" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17:I20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="23" customWidth="1"/>
+    <col min="2" max="2" width="22.33203125" customWidth="1"/>
+    <col min="3" max="3" width="26.33203125" customWidth="1"/>
+    <col min="4" max="4" width="19.88671875" customWidth="1"/>
+    <col min="5" max="5" width="17" customWidth="1"/>
+    <col min="6" max="6" width="16.5546875" customWidth="1"/>
+    <col min="7" max="7" width="18.77734375" customWidth="1"/>
+    <col min="8" max="8" width="16.21875" customWidth="1"/>
+    <col min="9" max="9" width="15" customWidth="1"/>
+    <col min="11" max="11" width="15.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12">
+      <c r="A1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H1" t="s">
+        <v>62</v>
+      </c>
+      <c r="I1" t="s">
+        <v>63</v>
+      </c>
+      <c r="J1" t="s">
+        <v>64</v>
+      </c>
+      <c r="K1" t="s">
+        <v>65</v>
+      </c>
+      <c r="L1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2">
+        <v>788</v>
+      </c>
+      <c r="D2">
+        <v>11111</v>
+      </c>
+      <c r="E2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F2" t="s">
+        <v>70</v>
+      </c>
+      <c r="G2">
+        <v>77</v>
+      </c>
+      <c r="H2" t="s">
+        <v>71</v>
+      </c>
+      <c r="I2" t="s">
+        <v>72</v>
+      </c>
+      <c r="J2" t="s">
+        <v>73</v>
+      </c>
+      <c r="K2" t="s">
+        <v>67</v>
+      </c>
+      <c r="L2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C3">
+        <v>7525</v>
+      </c>
+      <c r="D3">
+        <v>22225</v>
+      </c>
+      <c r="E3" t="s">
+        <v>76</v>
+      </c>
+      <c r="F3" t="s">
+        <v>77</v>
+      </c>
+      <c r="G3">
+        <v>12</v>
+      </c>
+      <c r="H3" t="s">
+        <v>78</v>
+      </c>
+      <c r="I3" t="s">
+        <v>79</v>
+      </c>
+      <c r="J3" t="s">
+        <v>80</v>
+      </c>
+      <c r="K3" t="s">
+        <v>67</v>
+      </c>
+      <c r="L3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C4">
+        <v>25488</v>
+      </c>
+      <c r="D4">
+        <v>99995</v>
+      </c>
+      <c r="E4" t="s">
+        <v>83</v>
+      </c>
+      <c r="F4" t="s">
+        <v>70</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4" t="s">
+        <v>84</v>
+      </c>
+      <c r="I4" t="s">
+        <v>85</v>
+      </c>
+      <c r="J4" t="s">
+        <v>73</v>
+      </c>
+      <c r="K4" t="s">
+        <v>67</v>
+      </c>
+      <c r="L4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C5">
+        <v>44525</v>
+      </c>
+      <c r="D5">
+        <v>55555</v>
+      </c>
+      <c r="E5" t="s">
+        <v>87</v>
+      </c>
+      <c r="F5" t="s">
+        <v>77</v>
+      </c>
+      <c r="G5">
+        <v>56</v>
+      </c>
+      <c r="H5" t="s">
+        <v>71</v>
+      </c>
+      <c r="I5" t="s">
+        <v>88</v>
+      </c>
+      <c r="J5" t="s">
+        <v>80</v>
+      </c>
+      <c r="K5" t="s">
+        <v>67</v>
+      </c>
+      <c r="L5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>